<commit_message>
csv folder for Google Sheets
</commit_message>
<xml_diff>
--- a/ASTS.xlsx
+++ b/ASTS.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="76">
   <si>
     <t>Price</t>
   </si>
@@ -137,25 +137,6 @@
     <t>Total COGC</t>
   </si>
   <si>
-    <r>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Interest Income</t>
-    </r>
-  </si>
-  <si>
-    <t>Includes: interest income; interest expense; other income (expense), net</t>
-  </si>
-  <si>
     <t>Gross Margin</t>
   </si>
   <si>
@@ -177,24 +158,9 @@
     <t>Other</t>
   </si>
   <si>
-    <t>A/P</t>
-  </si>
-  <si>
-    <t>Accured Liabilities</t>
-  </si>
-  <si>
     <t>Contracts</t>
   </si>
   <si>
-    <t>Liabilities</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>L + SE</t>
-  </si>
-  <si>
     <t>Net Cash</t>
   </si>
   <si>
@@ -262,6 +228,42 @@
   </si>
   <si>
     <t>Q424</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>expenses went up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           </t>
+  </si>
+  <si>
+    <t>OCA</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>Accrued</t>
+  </si>
+  <si>
+    <t>Lease</t>
+  </si>
+  <si>
+    <t>Total Liabilities</t>
+  </si>
+  <si>
+    <t>Total Assets</t>
   </si>
 </sst>
 </file>
@@ -270,9 +272,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +306,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -367,7 +376,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -382,8 +391,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -407,15 +419,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -425,8 +437,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14276294" y="526676"/>
-          <a:ext cx="0" cy="7194177"/>
+          <a:off x="13615147" y="549088"/>
+          <a:ext cx="0" cy="9883588"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -773,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L15"/>
+  <dimension ref="B2:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -812,7 +824,7 @@
     </row>
     <row r="4" spans="2:12">
       <c r="B4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
@@ -836,7 +848,7 @@
         <v>45610</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
         <v>4</v>
@@ -855,14 +867,30 @@
         <v>6450.4051100000006</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="15">
+    <row r="14" spans="2:12">
+      <c r="I14">
+        <v>2024</v>
+      </c>
       <c r="J14" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="J15" t="s">
-        <v>34</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10">
+      <c r="J17" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -875,13 +903,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB62"/>
+  <dimension ref="A1:AB71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
+      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -895,7 +923,7 @@
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="3" customFormat="1">
@@ -946,7 +974,7 @@
         <v>14</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="U3" s="3">
         <v>2021</v>
@@ -1028,8 +1056,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="U4">
-        <f t="shared" ref="U4:U21" si="1">SUM(D4:F4)</f>
-        <v>17.628</v>
+        <v>12.404999999999999</v>
+      </c>
+      <c r="V4">
+        <v>13.824999999999999</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -1080,8 +1113,13 @@
         <v>0</v>
       </c>
       <c r="U5">
-        <f t="shared" si="1"/>
-        <v>-10.778</v>
+        <v>7.5629999999999997</v>
+      </c>
+      <c r="V5">
+        <v>6.7140000000000004</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:28">
@@ -1098,27 +1136,27 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="F6" s="14">
-        <f t="shared" ref="F6:K6" si="2">F5+F4</f>
+        <f t="shared" ref="F6:K6" si="1">F5+F4</f>
         <v>4.8419999999999996</v>
       </c>
       <c r="G6" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.40800000000000014</v>
       </c>
       <c r="H6" s="14">
-        <f t="shared" si="2"/>
+        <f>H5+H4</f>
         <v>5.0620000000000003</v>
       </c>
       <c r="I6" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6430000000000002</v>
       </c>
       <c r="J6" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.1109999999999989</v>
       </c>
       <c r="K6" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L6" s="14">
@@ -1132,21 +1170,34 @@
         <v>0</v>
       </c>
       <c r="O6" s="14">
-        <f t="shared" ref="O6:Q6" si="3">O5+O4</f>
+        <f t="shared" ref="O6:Q6" si="2">O5+O4</f>
         <v>500</v>
       </c>
       <c r="P6" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="Q6" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="U6">
-        <f t="shared" si="1"/>
-        <v>6.85</v>
-      </c>
+      <c r="U6" s="14">
+        <f>U4-U5</f>
+        <v>4.8419999999999996</v>
+      </c>
+      <c r="V6" s="14">
+        <f>V4-V5</f>
+        <v>7.1109999999999989</v>
+      </c>
+      <c r="W6" s="14">
+        <f>W4-W5</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
     </row>
     <row r="7" spans="1:28">
       <c r="B7" s="5" t="s">
@@ -1195,10 +1246,20 @@
       <c r="Q7" s="14">
         <v>21.827999999999999</v>
       </c>
-      <c r="U7">
-        <f t="shared" si="1"/>
-        <v>43.945999999999998</v>
-      </c>
+      <c r="U7" s="14">
+        <v>29.599</v>
+      </c>
+      <c r="V7" s="14">
+        <v>54.212000000000003</v>
+      </c>
+      <c r="W7" s="14">
+        <v>78.811000000000007</v>
+      </c>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
     </row>
     <row r="8" spans="1:28">
       <c r="B8" s="5" t="s">
@@ -1247,10 +1308,20 @@
       <c r="Q8" s="14">
         <v>15.551</v>
       </c>
-      <c r="U8">
-        <f t="shared" si="1"/>
-        <v>54.124000000000002</v>
-      </c>
+      <c r="U8" s="14">
+        <v>35.636000000000003</v>
+      </c>
+      <c r="V8" s="14">
+        <v>48.332000000000001</v>
+      </c>
+      <c r="W8" s="14">
+        <v>41.600999999999999</v>
+      </c>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
     </row>
     <row r="9" spans="1:28">
       <c r="B9" s="5" t="s">
@@ -1299,10 +1370,20 @@
       <c r="Q9" s="14">
         <v>14.724</v>
       </c>
-      <c r="U9">
-        <f t="shared" si="1"/>
-        <v>37.380000000000003</v>
-      </c>
+      <c r="U9" s="14">
+        <v>23.44</v>
+      </c>
+      <c r="V9" s="14">
+        <v>45.62</v>
+      </c>
+      <c r="W9" s="14">
+        <v>47.485999999999997</v>
+      </c>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
     </row>
     <row r="10" spans="1:28">
       <c r="B10" s="5" t="s">
@@ -1351,10 +1432,20 @@
       <c r="Q10" s="14">
         <v>14.542999999999999</v>
       </c>
-      <c r="U10">
-        <f t="shared" si="1"/>
-        <v>4.3469999999999995</v>
-      </c>
+      <c r="U10" s="14">
+        <v>2.9129999999999998</v>
+      </c>
+      <c r="V10" s="14">
+        <v>4.7110000000000003</v>
+      </c>
+      <c r="W10" s="14">
+        <v>54.469000000000001</v>
+      </c>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
+      <c r="AB10" s="14"/>
     </row>
     <row r="11" spans="1:28">
       <c r="B11" s="5" t="s">
@@ -1362,69 +1453,82 @@
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14">
-        <f t="shared" ref="D11:P11" si="4">+D10+D9+D8+D7</f>
+        <f t="shared" ref="D11:P11" si="3">+D10+D9+D8+D7</f>
         <v>25.097000000000001</v>
       </c>
       <c r="E11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23.111999999999998</v>
       </c>
       <c r="F11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>91.588000000000008</v>
       </c>
       <c r="G11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>32.74</v>
       </c>
       <c r="H11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35.404000000000003</v>
       </c>
       <c r="I11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>42.123000000000005</v>
       </c>
       <c r="J11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>152.875</v>
       </c>
       <c r="K11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>44.454000000000001</v>
       </c>
       <c r="L11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>58.070000000000007</v>
       </c>
       <c r="M11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>58.965000000000003</v>
       </c>
       <c r="N11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>222.36699999999999</v>
       </c>
       <c r="O11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>55.988999999999997</v>
       </c>
       <c r="P11" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>63.893000000000001</v>
       </c>
       <c r="Q11" s="14">
         <f>+Q10+Q9+Q8+Q7</f>
         <v>66.646000000000001</v>
       </c>
-      <c r="U11">
-        <f t="shared" si="1"/>
-        <v>139.79700000000003</v>
-      </c>
+      <c r="U11" s="14">
+        <f>+U10+U9+U8+U7</f>
+        <v>91.588000000000008</v>
+      </c>
+      <c r="V11" s="14">
+        <f>+V10+V9+V8+V7</f>
+        <v>152.875</v>
+      </c>
+      <c r="W11" s="14">
+        <f>+W10+W9+W8+W7</f>
+        <v>222.36699999999999</v>
+      </c>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
     </row>
     <row r="12" spans="1:28">
       <c r="B12" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -1451,10 +1555,24 @@
       <c r="Q12" s="14">
         <v>-236.91200000000001</v>
       </c>
+      <c r="U12" s="14">
+        <v>15.766</v>
+      </c>
+      <c r="V12" s="14">
+        <v>19.114000000000001</v>
+      </c>
+      <c r="W12" s="14">
+        <v>8.9860000000000007</v>
+      </c>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
     </row>
     <row r="13" spans="1:28">
       <c r="B13" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1481,10 +1599,24 @@
       <c r="Q13" s="14">
         <v>-1.3859999999999999</v>
       </c>
+      <c r="U13" s="14">
+        <v>0</v>
+      </c>
+      <c r="V13" s="14">
+        <v>2.633</v>
+      </c>
+      <c r="W13" s="14">
+        <v>2.6749999999999998</v>
+      </c>
+      <c r="X13" s="14"/>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="14"/>
     </row>
     <row r="14" spans="1:28">
       <c r="B14" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -1511,6 +1643,20 @@
       <c r="Q14" s="14">
         <v>1.41</v>
       </c>
+      <c r="U14" s="14">
+        <v>-1.95</v>
+      </c>
+      <c r="V14" s="14">
+        <v>21.521000000000001</v>
+      </c>
+      <c r="W14" s="14">
+        <v>-10.29</v>
+      </c>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
     </row>
     <row r="15" spans="1:28">
       <c r="B15" s="5" t="s">
@@ -1564,14 +1710,27 @@
         <f>SUM(Q12:Q14)</f>
         <v>-236.88800000000001</v>
       </c>
-      <c r="U15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="U15" s="15">
+        <f>SUM(U12:U14)</f>
+        <v>13.816000000000001</v>
+      </c>
+      <c r="V15" s="15">
+        <f>SUM(V12:V14)</f>
+        <v>43.268000000000001</v>
+      </c>
+      <c r="W15" s="15">
+        <f>SUM(W12:W14)</f>
+        <v>1.3710000000000022</v>
+      </c>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
     </row>
     <row r="16" spans="1:28">
       <c r="B16" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1598,10 +1757,24 @@
       <c r="Q16" s="15">
         <v>-302.43400000000003</v>
       </c>
-    </row>
-    <row r="17" spans="2:21">
+      <c r="U16" s="15">
+        <v>-72.930000000000007</v>
+      </c>
+      <c r="V16" s="15">
+        <v>-102.496</v>
+      </c>
+      <c r="W16" s="15">
+        <v>-220.99600000000001</v>
+      </c>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+    </row>
+    <row r="17" spans="2:28">
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1628,10 +1801,24 @@
       <c r="Q17" s="15">
         <v>-0.64600000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="2:21">
+      <c r="U17" s="15">
+        <v>-0.33100000000000002</v>
+      </c>
+      <c r="V17" s="15">
+        <v>-0.61699999999999999</v>
+      </c>
+      <c r="W17" s="15">
+        <v>-1.681</v>
+      </c>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+    </row>
+    <row r="18" spans="2:28">
       <c r="B18" s="12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15">
@@ -1690,14 +1877,27 @@
         <f>SUM(Q16:Q17)</f>
         <v>-303.08000000000004</v>
       </c>
-      <c r="U18">
-        <f t="shared" si="1"/>
-        <v>-121.626</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21">
+      <c r="U18" s="15">
+        <f>SUM(U16:U17)</f>
+        <v>-73.26100000000001</v>
+      </c>
+      <c r="V18" s="15">
+        <f>SUM(V16:V17)</f>
+        <v>-103.113</v>
+      </c>
+      <c r="W18" s="15">
+        <f>SUM(W16:W17)</f>
+        <v>-222.67700000000002</v>
+      </c>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+    </row>
+    <row r="19" spans="2:28">
       <c r="B19" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15">
@@ -1743,14 +1943,24 @@
       <c r="Q19" s="15">
         <v>-131.13399999999999</v>
       </c>
-      <c r="U19">
-        <f t="shared" si="1"/>
-        <v>15.172000000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21">
+      <c r="U19" s="15">
+        <v>-42.707999999999998</v>
+      </c>
+      <c r="V19" s="15">
+        <v>-71.472999999999999</v>
+      </c>
+      <c r="W19" s="15">
+        <v>-135.11600000000001</v>
+      </c>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+    </row>
+    <row r="20" spans="2:28">
       <c r="B20" s="11" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15">
@@ -1800,12 +2010,25 @@
         <f>+Q18-Q19</f>
         <v>-171.94600000000005</v>
       </c>
-      <c r="U20">
-        <f t="shared" si="1"/>
-        <v>-46.416000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21">
+      <c r="U20" s="15">
+        <f>+U18-U19</f>
+        <v>-30.553000000000011</v>
+      </c>
+      <c r="V20" s="15">
+        <f>+V18-V19</f>
+        <v>-31.64</v>
+      </c>
+      <c r="W20" s="15">
+        <f>+W18-W19</f>
+        <v>-87.561000000000007</v>
+      </c>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+    </row>
+    <row r="21" spans="2:28">
       <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
@@ -1855,12 +2078,25 @@
         <f>+Q20/Q22</f>
         <v>-1.1047327169524517</v>
       </c>
-      <c r="U21">
-        <f t="shared" si="1"/>
-        <v>-0.67999999999999994</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21">
+      <c r="U21" s="13">
+        <f>+U20/U22</f>
+        <v>-0.5906268506625344</v>
+      </c>
+      <c r="V21" s="13">
+        <f>+V20/V22</f>
+        <v>-0.58122155098236095</v>
+      </c>
+      <c r="W21" s="13">
+        <f>+W20/W22</f>
+        <v>-1.0701123074684504</v>
+      </c>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+    </row>
+    <row r="22" spans="2:28">
       <c r="B22" s="5" t="s">
         <v>1</v>
       </c>
@@ -1907,52 +2143,80 @@
       <c r="Q22" s="2">
         <v>155.64488800000001</v>
       </c>
-      <c r="U22">
-        <f>AVERAGE(D22:F22)</f>
-        <v>51.729000000000006</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21">
+      <c r="U22" s="2">
+        <v>51.729785</v>
+      </c>
+      <c r="V22" s="2">
+        <v>54.437072999999998</v>
+      </c>
+      <c r="W22" s="2">
+        <v>81.824122000000003</v>
+      </c>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+    </row>
+    <row r="24" spans="2:28">
       <c r="B24" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6">
-        <f>H4/D4-1</f>
+        <f>IFERROR(H4/D4 -1, 0)</f>
         <v>1.6195456184637576</v>
       </c>
       <c r="I24" s="6">
-        <f>I4/E4-1</f>
+        <f>IFERROR(I4/E4 -1, 0)</f>
         <v>0.70122448979591834</v>
       </c>
+      <c r="J24" s="6">
+        <f>IFERROR(J4/F4 -1, 0)</f>
+        <v>0.11446997178557039</v>
+      </c>
       <c r="K24" s="6">
-        <f>K4/G4</f>
-        <v>0</v>
+        <f>IFERROR(K4/G4 -1, 0)</f>
+        <v>-1</v>
       </c>
       <c r="L24" s="6">
-        <v>0</v>
+        <f>IFERROR(L4/H4 -1, 0)</f>
+        <v>-1</v>
       </c>
       <c r="M24" s="6">
-        <v>0</v>
+        <f>IFERROR(M4/I4 -1, 0)</f>
+        <v>-1</v>
       </c>
       <c r="N24" s="6">
-        <f>N4/J4</f>
-        <v>0</v>
+        <f>IFERROR(N4/J4 -1, 0)</f>
+        <v>-1</v>
       </c>
       <c r="O24" s="6">
-        <v>5</v>
+        <f>IFERROR(O4/K4 -1, 0)</f>
+        <v>0</v>
       </c>
       <c r="P24" s="6">
-        <v>9</v>
+        <f>IFERROR(P4/L4 -1, 0)</f>
+        <v>0</v>
       </c>
       <c r="Q24" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21">
+        <f>IFERROR(Q4/M4 -1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U24" s="18"/>
+      <c r="V24" s="18">
+        <f>V4/U4</f>
+        <v>1.1144699717855704</v>
+      </c>
+      <c r="W24" s="18">
+        <f>W4/V4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28">
       <c r="B25" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F25" s="6">
         <f>F6/F4</f>
@@ -1970,6 +2234,10 @@
         <f>I6/I4</f>
         <v>0.39419385796545109</v>
       </c>
+      <c r="J25" s="6">
+        <f>J6/J4</f>
+        <v>0.51435804701627486</v>
+      </c>
       <c r="K25" s="6">
         <v>0</v>
       </c>
@@ -1994,619 +2262,844 @@
         <f>Q6/Q4</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:21">
+      <c r="U25" s="6">
+        <f>IFERROR(U6/U4, 0)</f>
+        <v>0.39032648125755742</v>
+      </c>
+      <c r="V25" s="6">
+        <f>IFERROR(V6/V4, 0)</f>
+        <v>0.51435804701627486</v>
+      </c>
+      <c r="W25" s="6">
+        <f>IFERROR(W6/W4, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28">
       <c r="B28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="P28" s="2">
-        <f>P45-P56</f>
-        <v>87763</v>
-      </c>
-      <c r="Q28" s="9"/>
-    </row>
-    <row r="29" spans="2:21">
+        <v>41</v>
+      </c>
+      <c r="O28" s="9">
+        <f>+O30-O42</f>
+        <v>51.358000000000033</v>
+      </c>
+      <c r="P28" s="9">
+        <f>+P30-P42</f>
+        <v>87.763000000000005</v>
+      </c>
+      <c r="Q28" s="9">
+        <f>+Q30-Q42</f>
+        <v>317.99899999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28">
+      <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="9"/>
     </row>
-    <row r="30" spans="2:21">
+    <row r="30" spans="2:28">
       <c r="B30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15">
+        <v>3</v>
+      </c>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15">
+        <f>209.973+2.467</f>
+        <v>212.44000000000003</v>
+      </c>
+      <c r="P30" s="15">
+        <f>285.085+2.482</f>
+        <v>287.56700000000001</v>
+      </c>
+      <c r="Q30" s="15">
+        <f>516.389+2.497</f>
+        <v>518.88599999999997</v>
+      </c>
+      <c r="V30">
+        <f>238.588+0.688</f>
+        <v>239.27599999999998</v>
+      </c>
+      <c r="W30">
+        <f>85.622+2.475</f>
+        <v>88.096999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28">
+      <c r="B31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15">
+        <v>5.0330000000000004</v>
+      </c>
+      <c r="P31" s="15">
+        <v>7.359</v>
+      </c>
+      <c r="Q31" s="15">
+        <v>7.0730000000000004</v>
+      </c>
+      <c r="V31">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W31">
+        <v>4.5910000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28">
+      <c r="B32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15">
+        <v>22.036000000000001</v>
+      </c>
+      <c r="P32" s="15">
+        <v>20.233000000000001</v>
+      </c>
+      <c r="Q32" s="15">
+        <v>19.661999999999999</v>
+      </c>
+      <c r="V32">
+        <v>24.954000000000001</v>
+      </c>
+      <c r="W32">
+        <v>14.194000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23">
+      <c r="B33" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15">
+        <v>245.28399999999999</v>
+      </c>
+      <c r="P33" s="15">
+        <v>248.16200000000001</v>
+      </c>
+      <c r="Q33" s="15">
+        <v>260.06799999999998</v>
+      </c>
+      <c r="V33">
+        <v>145.989</v>
+      </c>
+      <c r="W33">
+        <v>238.47800000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:23">
+      <c r="B34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15">
+        <v>12.795999999999999</v>
+      </c>
+      <c r="P34" s="15">
+        <v>12.343999999999999</v>
+      </c>
+      <c r="Q34" s="15">
+        <v>12.087999999999999</v>
+      </c>
+      <c r="V34">
+        <v>7.6710000000000003</v>
+      </c>
+      <c r="W34">
+        <v>13.221</v>
+      </c>
+    </row>
+    <row r="35" spans="2:23">
+      <c r="B35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15">
+        <v>4.1390000000000002</v>
+      </c>
+      <c r="P35" s="15">
+        <v>3.972</v>
+      </c>
+      <c r="Q35" s="15">
+        <v>3.8719999999999999</v>
+      </c>
+      <c r="V35">
+        <v>16.402000000000001</v>
+      </c>
+      <c r="W35">
+        <v>2.3109999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:23" ht="15">
+      <c r="B36" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="17">
+        <f>SUM(O30:O35)</f>
+        <v>501.72800000000001</v>
+      </c>
+      <c r="P36" s="17">
+        <f>SUM(P30:P35)</f>
+        <v>579.63700000000006</v>
+      </c>
+      <c r="Q36" s="17">
+        <f>SUM(Q30:Q35)</f>
+        <v>821.64899999999989</v>
+      </c>
+      <c r="V36" s="17">
+        <f>SUM(V30:V35)</f>
+        <v>438.39199999999994</v>
+      </c>
+      <c r="W36" s="17">
+        <f>SUM(W30:W35)</f>
+        <v>360.892</v>
+      </c>
+    </row>
+    <row r="37" spans="2:23">
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+    </row>
+    <row r="38" spans="2:23">
+      <c r="B38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15">
+        <v>14.528</v>
+      </c>
+      <c r="P38" s="15">
+        <v>12.175000000000001</v>
+      </c>
+      <c r="Q38" s="15">
+        <v>8.9619999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="2:23">
+      <c r="B39" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15">
+        <v>15.593</v>
+      </c>
+      <c r="P39" s="15">
+        <v>13.653</v>
+      </c>
+      <c r="Q39" s="15">
+        <v>16.48</v>
+      </c>
+    </row>
+    <row r="40" spans="2:23">
+      <c r="B40" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15">
+        <f>11.746</f>
+        <v>11.746</v>
+      </c>
+      <c r="P40" s="15">
+        <f>21.78+77.886</f>
+        <v>99.665999999999997</v>
+      </c>
+      <c r="Q40" s="15">
+        <f>22.468+57.46</f>
+        <v>79.927999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23">
+      <c r="B41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15">
+        <f>1.505+11.429</f>
+        <v>12.934000000000001</v>
+      </c>
+      <c r="P41" s="15">
+        <f>10.952+1.517</f>
+        <v>12.468999999999999</v>
+      </c>
+      <c r="Q41" s="15">
+        <f>1.534+11.057</f>
+        <v>12.591000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23">
+      <c r="B42" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15">
+        <f>0.255+160.827</f>
+        <v>161.08199999999999</v>
+      </c>
+      <c r="P42" s="15">
+        <f>0.258+199.546</f>
+        <v>199.804</v>
+      </c>
+      <c r="Q42" s="15">
+        <f>44.635+156.252</f>
+        <v>200.887</v>
+      </c>
+    </row>
+    <row r="43" spans="2:23" ht="15">
+      <c r="B43" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="17">
+        <f>SUM(O38:O42)</f>
+        <v>215.88299999999998</v>
+      </c>
+      <c r="P43" s="17">
+        <f>SUM(P38:P42)</f>
+        <v>337.767</v>
+      </c>
+      <c r="Q43" s="17">
+        <f>SUM(Q38:Q42)</f>
+        <v>318.84800000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:23">
+      <c r="B44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="9"/>
+    </row>
+    <row r="45" spans="2:23">
+      <c r="B45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15">
         <f>K18</f>
         <v>-45.216000000000001</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L45" s="15">
         <f>L18</f>
         <v>-49.588999999999999</v>
       </c>
-      <c r="M30" s="15">
+      <c r="M45" s="15">
         <f>M18</f>
         <v>-50.747999999999998</v>
       </c>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15">
+      <c r="N45" s="15"/>
+      <c r="O45" s="15">
         <f>O18</f>
         <v>-39.803999999999995</v>
       </c>
-      <c r="P30" s="15">
+      <c r="P45" s="15">
         <f>P18</f>
         <v>-131.35</v>
       </c>
-      <c r="Q30" s="15">
+      <c r="Q45" s="15">
         <f>Q18</f>
         <v>-303.08000000000004</v>
       </c>
     </row>
-    <row r="31" spans="2:21">
-      <c r="B31" s="5" t="s">
+    <row r="46" spans="2:23">
+      <c r="B46" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15">
+        <v>-45.216000000000001</v>
+      </c>
+      <c r="L46" s="15">
+        <f>-94.805-K46</f>
+        <v>-49.589000000000006</v>
+      </c>
+      <c r="M46" s="15">
+        <f>-145.553-L45-K45</f>
+        <v>-50.747999999999998</v>
+      </c>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15">
+        <v>-39.804000000000002</v>
+      </c>
+      <c r="P46" s="15">
+        <f>-171.154-O46</f>
+        <v>-131.35</v>
+      </c>
+      <c r="Q46" s="15">
+        <f>-474.234-P46-O46</f>
+        <v>-303.08000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="2:23">
+      <c r="B47" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15">
+        <v>1.7330000000000001</v>
+      </c>
+      <c r="L47" s="15">
+        <f>15.848-K47</f>
+        <v>14.115</v>
+      </c>
+      <c r="M47" s="15">
+        <f>34.877-L47-K47</f>
+        <v>19.029</v>
+      </c>
+      <c r="N47" s="15"/>
+      <c r="O47" s="15">
+        <v>19.945</v>
+      </c>
+      <c r="P47" s="15">
+        <f>40.336-O47</f>
+        <v>20.390999999999998</v>
+      </c>
+      <c r="Q47" s="15">
+        <f>54.88-P47-O47</f>
+        <v>14.544000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="2:23">
+      <c r="B48" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15">
+        <v>0</v>
+      </c>
+      <c r="L48" s="15">
+        <v>0</v>
+      </c>
+      <c r="M48" s="15">
+        <f>0.374-L48-K48</f>
+        <v>0.374</v>
+      </c>
+      <c r="N48" s="15"/>
+      <c r="O48" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="P48" s="15">
+        <f>1.901-O48</f>
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="Q48" s="15">
+        <f>3.047-P48-O48</f>
+        <v>1.1460000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17">
+      <c r="B49" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15">
+        <v>0</v>
+      </c>
+      <c r="M49" s="15">
+        <v>0</v>
+      </c>
+      <c r="N49" s="15"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15">
+        <v>2.2210000000000001</v>
+      </c>
+      <c r="Q49" s="15">
+        <f>2.221-P49-O49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17">
+      <c r="B50" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15">
+        <v>-7.4980000000000002</v>
+      </c>
+      <c r="L50" s="15">
+        <f>-13.973-K50</f>
+        <v>-6.4750000000000005</v>
+      </c>
+      <c r="M50" s="15">
+        <f>-21.454-L50-K50</f>
+        <v>-7.480999999999999</v>
+      </c>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15">
+        <v>-18.213999999999999</v>
+      </c>
+      <c r="P50" s="15">
+        <f>47.926+O50</f>
+        <v>29.712000000000003</v>
+      </c>
+      <c r="Q50" s="15">
+        <f>284.839-P50-O50</f>
+        <v>273.34100000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17">
+      <c r="B51" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15">
-        <v>-45.216000000000001</v>
-      </c>
-      <c r="L31" s="15">
-        <f>-94.805-K31</f>
-        <v>-49.589000000000006</v>
-      </c>
-      <c r="M31" s="15">
-        <f>-145.553-L30-K30</f>
-        <v>-50.747999999999998</v>
-      </c>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15">
-        <v>-39.804000000000002</v>
-      </c>
-      <c r="P31" s="15">
-        <f>-171.154-O31</f>
-        <v>-131.35</v>
-      </c>
-      <c r="Q31" s="15">
-        <f>-474.234-P31-O31</f>
-        <v>-303.08000000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21">
-      <c r="B32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15">
-        <v>1.7330000000000001</v>
-      </c>
-      <c r="L32" s="15">
-        <f>15.848-K32</f>
-        <v>14.115</v>
-      </c>
-      <c r="M32" s="15">
-        <f>34.877-L32-K32</f>
-        <v>19.029</v>
-      </c>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15">
-        <v>19.945</v>
-      </c>
-      <c r="P32" s="15">
-        <f>40.336-O32</f>
-        <v>20.390999999999998</v>
-      </c>
-      <c r="Q32" s="15">
-        <f>54.88-P32-O32</f>
-        <v>14.544000000000004</v>
-      </c>
-    </row>
-    <row r="33" spans="2:17">
-      <c r="B33" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15">
-        <v>0</v>
-      </c>
-      <c r="L33" s="15">
-        <v>0</v>
-      </c>
-      <c r="M33" s="15">
-        <f>0.374-L33-K33</f>
-        <v>0.374</v>
-      </c>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="P33" s="15">
-        <f>1.901-O33</f>
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="Q33" s="15">
-        <f>3.047-P33-O33</f>
-        <v>1.1460000000000004</v>
-      </c>
-    </row>
-    <row r="34" spans="2:17">
-      <c r="B34" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15">
-        <v>0</v>
-      </c>
-      <c r="M34" s="15">
-        <v>0</v>
-      </c>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="15">
-        <v>2.2210000000000001</v>
-      </c>
-      <c r="Q34" s="15">
-        <f>2.221-P34-O34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:17">
-      <c r="B35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15">
-        <v>-7.4980000000000002</v>
-      </c>
-      <c r="L35" s="15">
-        <f>-13.973-K35</f>
-        <v>-6.4750000000000005</v>
-      </c>
-      <c r="M35" s="15">
-        <f>-21.454-L35-K35</f>
-        <v>-7.480999999999999</v>
-      </c>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15">
-        <v>-18.213999999999999</v>
-      </c>
-      <c r="P35" s="15">
-        <f>47.926+O35</f>
-        <v>29.712000000000003</v>
-      </c>
-      <c r="Q35" s="15">
-        <f>284.839-P35-O35</f>
-        <v>273.34100000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="2:17">
-      <c r="B36" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15">
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15">
         <v>2.4740000000000002</v>
       </c>
-      <c r="L36" s="15">
-        <f>8.006-K36</f>
+      <c r="L51" s="15">
+        <f>8.006-K51</f>
         <v>5.532</v>
       </c>
-      <c r="M36" s="15">
-        <f>10.595-L36-K36</f>
+      <c r="M51" s="15">
+        <f>10.595-L51-K51</f>
         <v>2.5890000000000004</v>
       </c>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15">
+      <c r="N51" s="15"/>
+      <c r="O51" s="15">
         <v>4.9329999999999998</v>
       </c>
-      <c r="P36" s="15">
-        <f>13.807-O36</f>
+      <c r="P51" s="15">
+        <f>13.807-O51</f>
         <v>8.8740000000000006</v>
       </c>
-      <c r="Q36" s="15">
-        <f>20.617-P36-O36</f>
+      <c r="Q51" s="15">
+        <f>20.617-P51-O51</f>
         <v>6.8100000000000005</v>
       </c>
     </row>
-    <row r="37" spans="2:17">
-      <c r="B37" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15">
-        <v>0</v>
-      </c>
-      <c r="M37" s="15">
-        <v>0</v>
-      </c>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15">
+    <row r="52" spans="2:17">
+      <c r="B52" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15">
+        <v>0</v>
+      </c>
+      <c r="M52" s="15">
+        <v>0</v>
+      </c>
+      <c r="N52" s="15"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15">
         <v>2.9590000000000001</v>
       </c>
-      <c r="Q37" s="15">
-        <f>2.959-P37-O37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17">
-      <c r="B38" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15">
+      <c r="Q52" s="15">
+        <f>2.959-P52-O52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:17">
+      <c r="B53" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15">
         <f>-12.168+5.553+0.006+17.383</f>
         <v>10.774000000000001</v>
       </c>
-      <c r="L38" s="15">
-        <f>-15.547-4.112+0.035+0+16.559-K38</f>
+      <c r="L53" s="15">
+        <f>-15.547-4.112+0.035+0+16.559-K53</f>
         <v>-13.838999999999999</v>
       </c>
-      <c r="M38" s="15">
-        <f>1.601-6.215+0.054+0+1.68-L38-K38</f>
+      <c r="M53" s="15">
+        <f>1.601-6.215+0.054+0+1.68-L53-K53</f>
         <v>0.18499999999999872</v>
       </c>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15">
+      <c r="N53" s="15"/>
+      <c r="O53" s="15">
         <f>-8.306-8.396-0.008+0.828</f>
         <v>-15.881999999999998</v>
       </c>
-      <c r="P38" s="15">
-        <f>-10.128-14.873-(21/1000)+21.78+(972/1000)-O38</f>
+      <c r="P53" s="15">
+        <f>-10.128-14.873-(21/1000)+21.78+(972/1000)-O53</f>
         <v>13.612</v>
       </c>
-      <c r="Q38" s="15">
-        <f>7.94-7.998+0.357+22.468+1.081-P38-O38</f>
+      <c r="Q53" s="15">
+        <f>7.94-7.998+0.357+22.468+1.081-P53-O53</f>
         <v>26.117999999999995</v>
       </c>
     </row>
-    <row r="39" spans="2:17">
-      <c r="B39" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15">
-        <f>SUM(K31:K38)</f>
+    <row r="54" spans="2:17">
+      <c r="B54" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15">
+        <f>SUM(K46:K53)</f>
         <v>-37.733000000000004</v>
       </c>
-      <c r="L39" s="15">
-        <f>SUM(L31:L38)</f>
+      <c r="L54" s="15">
+        <f>SUM(L46:L53)</f>
         <v>-50.256</v>
       </c>
-      <c r="M39" s="15">
-        <f>SUM(M31:M38)</f>
+      <c r="M54" s="15">
+        <f>SUM(M46:M53)</f>
         <v>-36.052000000000007</v>
       </c>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15">
-        <f>SUM(O31:O38)</f>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15">
+        <f>SUM(O46:O53)</f>
         <v>-48.122</v>
       </c>
-      <c r="P39" s="15">
-        <f>SUM(P31:P38)</f>
+      <c r="P54" s="15">
+        <f>SUM(P46:P53)</f>
         <v>-52.579999999999991</v>
       </c>
-      <c r="Q39" s="15">
-        <f>SUM(Q31:Q38)</f>
+      <c r="Q54" s="15">
+        <f>SUM(Q46:Q53)</f>
         <v>18.878999999999962</v>
       </c>
     </row>
-    <row r="40" spans="2:17">
-      <c r="P40" s="2"/>
-      <c r="Q40" s="9"/>
-    </row>
-    <row r="41" spans="2:17">
-      <c r="B41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15">
+    <row r="55" spans="2:17">
+      <c r="P55" s="2"/>
+      <c r="Q55" s="9"/>
+    </row>
+    <row r="56" spans="2:17">
+      <c r="B56" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15">
         <v>-37.732999999999997</v>
       </c>
-      <c r="L41" s="15">
-        <f>-87.989-K41</f>
+      <c r="L56" s="15">
+        <f>-87.989-K56</f>
         <v>-50.256000000000007</v>
       </c>
-      <c r="M41" s="15">
-        <f>-124.041-L41-K41</f>
+      <c r="M56" s="15">
+        <f>-124.041-L56-K56</f>
         <v>-36.052</v>
       </c>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15">
+      <c r="N56" s="15"/>
+      <c r="O56" s="15">
         <v>-48.122</v>
       </c>
-      <c r="P41" s="15">
-        <f>-64.274-O41</f>
+      <c r="P56" s="15">
+        <f>-64.274-O56</f>
         <v>-16.152000000000001</v>
       </c>
-      <c r="Q41" s="9">
-        <f>-97.703-P41-O41</f>
+      <c r="Q56" s="9">
+        <f>-97.703-P56-O56</f>
         <v>-33.429000000000002</v>
       </c>
     </row>
-    <row r="42" spans="2:17">
-      <c r="B42" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15">
+    <row r="57" spans="2:17">
+      <c r="B57" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
+      <c r="K57" s="15">
         <v>-15.388</v>
       </c>
-      <c r="L42" s="15">
-        <f>-22.972-K42</f>
+      <c r="L57" s="15">
+        <f>-22.972-K57</f>
         <v>-7.5840000000000014</v>
       </c>
-      <c r="M42" s="15">
-        <f>-96.462-L42-K42</f>
+      <c r="M57" s="15">
+        <f>-96.462-L57-K57</f>
         <v>-73.489999999999995</v>
       </c>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15">
+      <c r="N57" s="15"/>
+      <c r="O57" s="15">
         <v>-39.567999999999998</v>
       </c>
-      <c r="P42" s="15">
-        <f>-61.77-O42</f>
+      <c r="P57" s="15">
+        <f>-61.77-O57</f>
         <v>-22.202000000000005</v>
       </c>
-      <c r="Q42" s="9">
-        <f>-92.095-P42-O42</f>
+      <c r="Q57" s="9">
+        <f>-92.095-P57-O57</f>
         <v>-30.325000000000003</v>
       </c>
     </row>
-    <row r="43" spans="2:17">
-      <c r="B43" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15">
-        <f>+K41-K42</f>
+    <row r="58" spans="2:17">
+      <c r="B58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15">
+        <f>+K56-K57</f>
         <v>-22.344999999999999</v>
       </c>
-      <c r="L43" s="15">
-        <f>+L41-L42</f>
+      <c r="L58" s="15">
+        <f>+L56-L57</f>
         <v>-42.672000000000004</v>
       </c>
-      <c r="M43" s="15">
-        <f>+M41-M42</f>
+      <c r="M58" s="15">
+        <f>+M56-M57</f>
         <v>37.437999999999995</v>
       </c>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15">
-        <f>+O41-O42</f>
+      <c r="N58" s="15"/>
+      <c r="O58" s="15">
+        <f>+O56-O57</f>
         <v>-8.554000000000002</v>
       </c>
-      <c r="P43" s="15">
-        <f>+P41+P42</f>
+      <c r="P58" s="15">
+        <f>+P56+P57</f>
         <v>-38.354000000000006</v>
       </c>
-      <c r="Q43" s="15">
-        <f>+Q41+Q42</f>
+      <c r="Q58" s="15">
+        <f>+Q56+Q57</f>
         <v>-63.754000000000005</v>
       </c>
     </row>
-    <row r="44" spans="2:17">
-      <c r="B44" s="8"/>
-      <c r="N44" s="15"/>
-    </row>
-    <row r="45" spans="2:17">
-      <c r="B45" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="N45" s="15"/>
-      <c r="P45" s="2">
-        <f>285085+2482</f>
-        <v>287567</v>
-      </c>
-    </row>
-    <row r="46" spans="2:17">
-      <c r="B46" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="P46" s="2">
-        <v>7359</v>
-      </c>
-    </row>
-    <row r="47" spans="2:17">
-      <c r="B47" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P47" s="2">
-        <f>20233+3972</f>
-        <v>24205</v>
-      </c>
-    </row>
-    <row r="48" spans="2:17">
-      <c r="B48" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P48">
-        <v>248162</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16">
-      <c r="B49" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="P49" s="2">
-        <v>12344</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16">
-      <c r="B50" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P50" s="2">
-        <f>SUM(P45:P49)</f>
-        <v>579637</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16">
-      <c r="B52" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P52" s="2">
-        <v>12175</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16">
-      <c r="B53" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="P53" s="2">
-        <v>13653</v>
-      </c>
-    </row>
-    <row r="54" spans="2:16">
-      <c r="B54" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="P54" s="2">
-        <f>21780+77886</f>
-        <v>99666</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16">
-      <c r="B55" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="P55" s="2">
-        <f>1517+10952</f>
-        <v>12469</v>
-      </c>
-    </row>
-    <row r="56" spans="2:16">
-      <c r="B56" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P56" s="2">
-        <f>258+199546</f>
-        <v>199804</v>
-      </c>
-    </row>
-    <row r="57" spans="2:16">
-      <c r="B57" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P57" s="2">
-        <f>SUM(P52:P56)</f>
-        <v>337767</v>
-      </c>
-    </row>
-    <row r="58" spans="2:16">
-      <c r="B58" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="P58" s="2">
-        <v>241870</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16">
-      <c r="B59" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="P59" s="2">
-        <f>SUM(P57:P58)</f>
-        <v>579637</v>
-      </c>
-    </row>
-    <row r="60" spans="2:16">
-      <c r="P60" s="2"/>
-    </row>
-    <row r="61" spans="2:16">
+    <row r="59" spans="2:17">
+      <c r="B59" s="8"/>
+      <c r="N59" s="15"/>
+    </row>
+    <row r="61" spans="2:17">
       <c r="P61" s="2"/>
     </row>
-    <row r="62" spans="2:16">
+    <row r="62" spans="2:17">
       <c r="P62" s="2"/>
+    </row>
+    <row r="63" spans="2:17">
+      <c r="P63" s="2"/>
+    </row>
+    <row r="64" spans="2:17">
+      <c r="P64" s="2"/>
+    </row>
+    <row r="65" spans="16:16">
+      <c r="P65" s="2"/>
+    </row>
+    <row r="66" spans="16:16">
+      <c r="P66" s="2"/>
+    </row>
+    <row r="67" spans="16:16">
+      <c r="P67" s="2"/>
+    </row>
+    <row r="68" spans="16:16">
+      <c r="P68" s="2"/>
+    </row>
+    <row r="69" spans="16:16">
+      <c r="P69" s="2"/>
+    </row>
+    <row r="70" spans="16:16">
+      <c r="P70" s="2"/>
+    </row>
+    <row r="71" spans="16:16">
+      <c r="P71" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated HON Q324, Q422
</commit_message>
<xml_diff>
--- a/ASTS.xlsx
+++ b/ASTS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u144455\OneDrive - Eastman Chemical Company\Desktop\personal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u144455\OneDrive - Eastman Chemical Company\Desktop\personal\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28275" yWindow="0" windowWidth="28095" windowHeight="14700" activeTab="1"/>
+    <workbookView xWindow="28275" yWindow="0" windowWidth="28095" windowHeight="14700"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -242,9 +242,6 @@
     <t>Q4</t>
   </si>
   <si>
-    <t>expenses went up</t>
-  </si>
-  <si>
     <t xml:space="preserve">           </t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>Total Assets</t>
+  </si>
+  <si>
+    <t>expenses went up (-); prepaids up (+)</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -885,7 +885,7 @@
         <v>66</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="10:10">
@@ -905,11 +905,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O19" sqref="O19"/>
+      <selection pane="bottomRight" activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2165,43 +2165,43 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6">
-        <f>IFERROR(H4/D4 -1, 0)</f>
+        <f t="shared" ref="H24:Q24" si="4">IFERROR(H4/D4 -1, 0)</f>
         <v>1.6195456184637576</v>
       </c>
       <c r="I24" s="6">
-        <f>IFERROR(I4/E4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>0.70122448979591834</v>
       </c>
       <c r="J24" s="6">
-        <f>IFERROR(J4/F4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>0.11446997178557039</v>
       </c>
       <c r="K24" s="6">
-        <f>IFERROR(K4/G4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="L24" s="6">
-        <f>IFERROR(L4/H4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="M24" s="6">
-        <f>IFERROR(M4/I4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="N24" s="6">
-        <f>IFERROR(N4/J4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="O24" s="6">
-        <f>IFERROR(O4/K4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P24" s="6">
-        <f>IFERROR(P4/L4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q24" s="6">
-        <f>IFERROR(Q4/M4 -1, 0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U24" s="18"/>
@@ -2350,7 +2350,7 @@
     </row>
     <row r="32" spans="2:28">
       <c r="B32" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="36" spans="2:23" ht="15">
       <c r="B36" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="38" spans="2:23">
       <c r="B38" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
@@ -2495,7 +2495,7 @@
     </row>
     <row r="39" spans="2:23">
       <c r="B39" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
@@ -2532,7 +2532,7 @@
     </row>
     <row r="41" spans="2:23">
       <c r="B41" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="43" spans="2:23" ht="15">
       <c r="B43" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J43" s="15"/>
       <c r="K43" s="15"/>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="44" spans="2:23">
       <c r="B44" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P44" s="2"/>
       <c r="Q44" s="9"/>

</xml_diff>